<commit_message>
baixado arquivos do struts
</commit_message>
<xml_diff>
--- a/1_2_vulnerabilidades_por_projeto.xlsx
+++ b/1_2_vulnerabilidades_por_projeto.xlsx
@@ -453,14 +453,14 @@
     <row r="2">
       <c r="A2" t="inlineStr">
         <is>
-          <t>systemd</t>
+          <t>Struts</t>
         </is>
       </c>
       <c r="B2" t="n">
-        <v>32</v>
+        <v>52</v>
       </c>
       <c r="C2" t="n">
-        <v>25</v>
+        <v>46</v>
       </c>
     </row>
   </sheetData>

</xml_diff>